<commit_message>
with open() refactor and updates
</commit_message>
<xml_diff>
--- a/data/output/~dicom_dicom_tags.xlsx
+++ b/data/output/~dicom_dicom_tags.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_Public_Examples\dicom_router_parser\data\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D1A46-E2EE-4A8F-AE10-6370A25721F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6105" yWindow="990" windowWidth="27990" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="~dicom_dicom_tags" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'~dicom_dicom_tags'!$A$1:$I$65536</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -169,8 +175,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +254,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -294,7 +308,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,9 +340,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,6 +392,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -535,28 +585,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -614,7 +664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -641,7 +691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -666,7 +716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -693,7 +743,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -720,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
@@ -748,7 +798,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I65536"/>
+  <autoFilter ref="A1:I65536" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="C2:C7">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="OT">
       <formula>NOT(ISERROR(SEARCH("OT",C2)))</formula>

</xml_diff>